<commit_message>
/ ‘Extended Campuses/Self Appraisals/2014/Raw Data from Database.xlsx’
</commit_message>
<xml_diff>
--- a/Extended Campuses/Self Appraisals/2014/Raw Data from Database.xlsx
+++ b/Extended Campuses/Self Appraisals/2014/Raw Data from Database.xlsx
@@ -2954,7 +2954,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3036,6 +3036,9 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3668,8 +3671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K830"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3742,7 +3745,9 @@
       <c r="H2" s="18">
         <v>1</v>
       </c>
-      <c r="I2" s="18"/>
+      <c r="I2" s="18">
+        <v>1</v>
+      </c>
       <c r="J2" s="18"/>
       <c r="K2" s="19"/>
     </row>
@@ -3759,13 +3764,15 @@
       <c r="D3" s="6" t="s">
         <v>744</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="34" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
+      <c r="I3" s="18">
+        <v>1</v>
+      </c>
       <c r="J3" s="18"/>
       <c r="K3" s="19"/>
     </row>
@@ -3792,7 +3799,9 @@
       <c r="H4" s="18">
         <v>1</v>
       </c>
-      <c r="I4" s="18"/>
+      <c r="I4" s="18">
+        <v>1</v>
+      </c>
       <c r="J4" s="18"/>
       <c r="K4" s="19"/>
     </row>
@@ -3815,7 +3824,9 @@
       <c r="F5" s="17"/>
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="I5" s="18">
+        <v>1</v>
+      </c>
       <c r="J5" s="18"/>
       <c r="K5" s="19"/>
     </row>
@@ -3838,7 +3849,9 @@
       <c r="F6" s="17"/>
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="I6" s="18">
+        <v>1</v>
+      </c>
       <c r="J6" s="18"/>
       <c r="K6" s="19"/>
     </row>
@@ -3861,7 +3874,9 @@
       <c r="F7" s="17"/>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="I7" s="18">
+        <v>1</v>
+      </c>
       <c r="J7" s="18"/>
       <c r="K7" s="19"/>
     </row>
@@ -3884,7 +3899,9 @@
       <c r="F8" s="17"/>
       <c r="G8" s="18"/>
       <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+      <c r="I8" s="18">
+        <v>1</v>
+      </c>
       <c r="J8" s="18"/>
       <c r="K8" s="19"/>
     </row>
@@ -3907,7 +3924,9 @@
       <c r="F9" s="17"/>
       <c r="G9" s="18"/>
       <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+      <c r="I9" s="18">
+        <v>1</v>
+      </c>
       <c r="J9" s="18"/>
       <c r="K9" s="19"/>
     </row>
@@ -3930,7 +3949,9 @@
       <c r="F10" s="17"/>
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
+      <c r="I10" s="18">
+        <v>1</v>
+      </c>
       <c r="J10" s="18"/>
       <c r="K10" s="19"/>
     </row>
@@ -4001,7 +4022,9 @@
       <c r="F13" s="17"/>
       <c r="G13" s="18"/>
       <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
+      <c r="I13" s="18">
+        <v>1</v>
+      </c>
       <c r="J13" s="18"/>
       <c r="K13" s="19"/>
     </row>
@@ -4024,7 +4047,9 @@
       <c r="F14" s="17"/>
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="I14" s="18">
+        <v>1</v>
+      </c>
       <c r="J14" s="18"/>
       <c r="K14" s="19"/>
     </row>
@@ -4047,7 +4072,9 @@
       <c r="F15" s="17"/>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
+      <c r="I15" s="18">
+        <v>1</v>
+      </c>
       <c r="J15" s="18"/>
       <c r="K15" s="19"/>
     </row>
@@ -4070,7 +4097,9 @@
       <c r="F16" s="17"/>
       <c r="G16" s="18"/>
       <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
+      <c r="I16" s="18">
+        <v>1</v>
+      </c>
       <c r="J16" s="18"/>
       <c r="K16" s="19"/>
     </row>
@@ -4093,7 +4122,9 @@
       <c r="F17" s="17"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
+      <c r="I17" s="18">
+        <v>1</v>
+      </c>
       <c r="J17" s="18"/>
       <c r="K17" s="19"/>
     </row>
@@ -4116,7 +4147,9 @@
       <c r="F18" s="17"/>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
+      <c r="I18" s="18">
+        <v>1</v>
+      </c>
       <c r="J18" s="18"/>
       <c r="K18" s="19"/>
     </row>
@@ -4139,7 +4172,9 @@
       <c r="F19" s="17"/>
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
+      <c r="I19" s="18">
+        <v>1</v>
+      </c>
       <c r="J19" s="18"/>
       <c r="K19" s="19"/>
     </row>
@@ -4208,7 +4243,9 @@
       <c r="F22" s="17"/>
       <c r="G22" s="18"/>
       <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
+      <c r="I22" s="18">
+        <v>1</v>
+      </c>
       <c r="J22" s="18"/>
       <c r="K22" s="19"/>
     </row>
@@ -4233,7 +4270,9 @@
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
+      <c r="K23" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
@@ -4254,9 +4293,13 @@
       <c r="F24" s="17"/>
       <c r="G24" s="18"/>
       <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
+      <c r="I24" s="18">
+        <v>1</v>
+      </c>
       <c r="J24" s="18"/>
-      <c r="K24" s="19"/>
+      <c r="K24" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
@@ -4277,9 +4320,13 @@
       <c r="F25" s="17"/>
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
+      <c r="I25" s="18">
+        <v>1</v>
+      </c>
       <c r="J25" s="18"/>
-      <c r="K25" s="19"/>
+      <c r="K25" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
@@ -4300,9 +4347,13 @@
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
+      <c r="I26" s="18">
+        <v>1</v>
+      </c>
       <c r="J26" s="18"/>
-      <c r="K26" s="19"/>
+      <c r="K26" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
@@ -4323,9 +4374,13 @@
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
       <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
+      <c r="I27" s="18">
+        <v>1</v>
+      </c>
       <c r="J27" s="18"/>
-      <c r="K27" s="19"/>
+      <c r="K27" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
@@ -4367,9 +4422,15 @@
         <v>433</v>
       </c>
       <c r="F29" s="17"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
+      <c r="G29" s="18">
+        <v>1</v>
+      </c>
+      <c r="H29" s="18">
+        <v>1</v>
+      </c>
+      <c r="I29" s="18">
+        <v>1</v>
+      </c>
       <c r="J29" s="18"/>
       <c r="K29" s="19"/>
     </row>
@@ -4505,9 +4566,13 @@
         <v>531</v>
       </c>
       <c r="F35" s="17"/>
-      <c r="G35" s="18"/>
+      <c r="G35" s="18">
+        <v>1</v>
+      </c>
       <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
+      <c r="I35" s="18">
+        <v>1</v>
+      </c>
       <c r="J35" s="18"/>
       <c r="K35" s="19"/>
     </row>
@@ -4666,9 +4731,13 @@
         <v>667</v>
       </c>
       <c r="F42" s="17"/>
-      <c r="G42" s="18"/>
+      <c r="G42" s="18">
+        <v>1</v>
+      </c>
       <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
+      <c r="I42" s="18">
+        <v>1</v>
+      </c>
       <c r="J42" s="18"/>
       <c r="K42" s="19"/>
     </row>
@@ -4758,9 +4827,13 @@
         <v>689</v>
       </c>
       <c r="F46" s="17"/>
-      <c r="G46" s="18"/>
+      <c r="G46" s="18">
+        <v>1</v>
+      </c>
       <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
+      <c r="I46" s="18">
+        <v>1</v>
+      </c>
       <c r="J46" s="18"/>
       <c r="K46" s="19"/>
     </row>
@@ -4831,7 +4904,9 @@
       <c r="H49" s="18"/>
       <c r="I49" s="18"/>
       <c r="J49" s="18"/>
-      <c r="K49" s="19"/>
+      <c r="K49" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="14">
@@ -4946,7 +5021,9 @@
       <c r="H54" s="25"/>
       <c r="I54" s="25"/>
       <c r="J54" s="25"/>
-      <c r="K54" s="26"/>
+      <c r="K54" s="26">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="20">
@@ -4969,7 +5046,9 @@
       <c r="H55" s="25"/>
       <c r="I55" s="25"/>
       <c r="J55" s="25"/>
-      <c r="K55" s="26"/>
+      <c r="K55" s="26">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="20">
@@ -4992,7 +5071,9 @@
       <c r="H56" s="25"/>
       <c r="I56" s="25"/>
       <c r="J56" s="25"/>
-      <c r="K56" s="26"/>
+      <c r="K56" s="26">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="20">
@@ -5015,7 +5096,9 @@
       <c r="H57" s="25"/>
       <c r="I57" s="25"/>
       <c r="J57" s="25"/>
-      <c r="K57" s="26"/>
+      <c r="K57" s="26">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="20">
@@ -5038,7 +5121,9 @@
       <c r="H58" s="25"/>
       <c r="I58" s="25"/>
       <c r="J58" s="25"/>
-      <c r="K58" s="26"/>
+      <c r="K58" s="26">
+        <v>1</v>
+      </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="20">
@@ -5061,7 +5146,9 @@
       <c r="H59" s="25"/>
       <c r="I59" s="25"/>
       <c r="J59" s="25"/>
-      <c r="K59" s="26"/>
+      <c r="K59" s="26">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="14">

</xml_diff>

<commit_message>
/ ‘Extended Campuses/Self Appraisals/2014/Raw Data from Database.xlsx’ / ‘Extended Campuses/Self Appraisals/2014/Talbert_Tso_ASA_PA_2013-14.doc’
</commit_message>
<xml_diff>
--- a/Extended Campuses/Self Appraisals/2014/Raw Data from Database.xlsx
+++ b/Extended Campuses/Self Appraisals/2014/Raw Data from Database.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -2960,7 +2960,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3048,6 +3048,12 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3815,8 +3821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K830"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E161" workbookViewId="0">
-      <selection activeCell="G171" sqref="G171"/>
+    <sheetView tabSelected="1" topLeftCell="E173" workbookViewId="0">
+      <selection activeCell="K167" sqref="K167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8047,10 +8053,10 @@
       <c r="E167" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F167" s="17">
-        <v>1</v>
-      </c>
-      <c r="G167" s="18"/>
+      <c r="F167" s="17"/>
+      <c r="G167" s="36">
+        <v>2</v>
+      </c>
       <c r="H167" s="18"/>
       <c r="I167" s="18"/>
       <c r="J167" s="18"/>
@@ -8072,10 +8078,10 @@
       <c r="E168" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F168" s="17">
-        <v>1</v>
-      </c>
-      <c r="G168" s="18"/>
+      <c r="F168" s="17"/>
+      <c r="G168" s="36">
+        <v>2</v>
+      </c>
       <c r="H168" s="18"/>
       <c r="I168" s="18"/>
       <c r="J168" s="18"/>
@@ -8097,10 +8103,10 @@
       <c r="E169" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F169" s="17">
-        <v>1</v>
-      </c>
-      <c r="G169" s="18"/>
+      <c r="F169" s="17"/>
+      <c r="G169" s="36">
+        <v>2</v>
+      </c>
       <c r="H169" s="18"/>
       <c r="I169" s="18"/>
       <c r="J169" s="18"/>
@@ -8123,7 +8129,7 @@
         <v>132</v>
       </c>
       <c r="F170" s="24"/>
-      <c r="G170" s="25"/>
+      <c r="G170" s="37"/>
       <c r="H170" s="25"/>
       <c r="I170" s="25"/>
       <c r="J170" s="25"/>
@@ -8145,10 +8151,10 @@
       <c r="E171" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F171" s="17">
-        <v>1</v>
-      </c>
-      <c r="G171" s="18"/>
+      <c r="F171" s="17"/>
+      <c r="G171" s="36">
+        <v>2</v>
+      </c>
       <c r="H171" s="18"/>
       <c r="I171" s="18"/>
       <c r="J171" s="18"/>
@@ -8170,10 +8176,10 @@
       <c r="E172" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F172" s="17">
-        <v>1</v>
-      </c>
-      <c r="G172" s="18"/>
+      <c r="F172" s="17"/>
+      <c r="G172" s="36">
+        <v>2</v>
+      </c>
       <c r="H172" s="18"/>
       <c r="I172" s="18"/>
       <c r="J172" s="18"/>
@@ -8195,10 +8201,10 @@
       <c r="E173" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="F173" s="17">
-        <v>1</v>
-      </c>
-      <c r="G173" s="18"/>
+      <c r="F173" s="17"/>
+      <c r="G173" s="36">
+        <v>2</v>
+      </c>
       <c r="H173" s="18"/>
       <c r="I173" s="18"/>
       <c r="J173" s="18"/>

</xml_diff>

<commit_message>
/ ‘Extended Campuses/Self Appraisals/2014/Raw Data from Database.xlsx’ / ‘Extended Campuses/Self Appraisals/2014/Talbert_Tso_ASA_PA_2013-14.doc’ + ‘Extended Campuses/Self Appraisals/2014/D851A410’
</commit_message>
<xml_diff>
--- a/Extended Campuses/Self Appraisals/2014/Raw Data from Database.xlsx
+++ b/Extended Campuses/Self Appraisals/2014/Raw Data from Database.xlsx
@@ -3826,8 +3826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K830"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A602" workbookViewId="0">
-      <selection activeCell="K607" sqref="K607"/>
+    <sheetView tabSelected="1" topLeftCell="A638" workbookViewId="0">
+      <selection activeCell="G618" sqref="G618"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19413,7 +19413,7 @@
       <c r="E616" s="6" t="s">
         <v>550</v>
       </c>
-      <c r="F616" s="17">
+      <c r="F616" s="35">
         <v>1</v>
       </c>
       <c r="G616" s="18"/>
@@ -19438,7 +19438,7 @@
       <c r="E617" s="6" t="s">
         <v>551</v>
       </c>
-      <c r="F617" s="17">
+      <c r="F617" s="35">
         <v>1</v>
       </c>
       <c r="G617" s="18"/>

</xml_diff>